<commit_message>
Played with xls, it changed
</commit_message>
<xml_diff>
--- a/systemic-base.xlsx
+++ b/systemic-base.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\OlivierThibot\4.GITHUB\systemic\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0130D3A8-8845-4A7C-9811-7E433ECA9653}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BCD0372-A335-4978-BA5C-1ED0D314ABAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-105" windowWidth="29040" windowHeight="16440" xr2:uid="{6D051935-CA26-4DED-98CB-D2D09C8C162C}"/>
+    <workbookView xWindow="28800" yWindow="15" windowWidth="8850" windowHeight="16200" activeTab="1" xr2:uid="{6D051935-CA26-4DED-98CB-D2D09C8C162C}"/>
   </bookViews>
   <sheets>
     <sheet name="nodes" sheetId="1" r:id="rId1"/>
     <sheet name="edges" sheetId="2" r:id="rId2"/>
+    <sheet name="backup" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="36">
   <si>
     <t>Node1</t>
   </si>
@@ -124,6 +125,27 @@
   </si>
   <si>
     <t>Pétrole</t>
+  </si>
+  <si>
+    <t>Innovation</t>
+  </si>
+  <si>
+    <t>Métaux</t>
+  </si>
+  <si>
+    <t>Plastiques</t>
+  </si>
+  <si>
+    <t>Enérgie</t>
+  </si>
+  <si>
+    <t>Pollution</t>
+  </si>
+  <si>
+    <t>Sobriété</t>
+  </si>
+  <si>
+    <t>Recyclage</t>
   </si>
 </sst>
 </file>
@@ -504,13 +526,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52D2128C-C535-4121-AE48-AB103AC1AFB4}">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="30.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="13.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
@@ -525,21 +551,21 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="C2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="C3" t="s">
         <v>23</v>
@@ -547,10 +573,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="C4" t="s">
         <v>23</v>
@@ -558,21 +584,21 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>29</v>
       </c>
       <c r="B5" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="C5" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="C6" t="s">
         <v>25</v>
@@ -580,111 +606,23 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="B7" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="C7" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>17</v>
+        <v>35</v>
       </c>
       <c r="B8" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="C8" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>3</v>
-      </c>
-      <c r="B9" t="s">
-        <v>22</v>
-      </c>
-      <c r="C9" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10" t="s">
-        <v>22</v>
-      </c>
-      <c r="C10" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" t="s">
-        <v>26</v>
-      </c>
-      <c r="C11" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12" t="s">
-        <v>24</v>
-      </c>
-      <c r="C12" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>11</v>
-      </c>
-      <c r="B13" t="s">
-        <v>22</v>
-      </c>
-      <c r="C13" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>18</v>
-      </c>
-      <c r="B14" t="s">
-        <v>27</v>
-      </c>
-      <c r="C14" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>16</v>
-      </c>
-      <c r="B15" t="s">
-        <v>24</v>
-      </c>
-      <c r="C15" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>28</v>
-      </c>
-      <c r="B16" t="s">
-        <v>24</v>
-      </c>
-      <c r="C16" t="s">
         <v>25</v>
       </c>
     </row>
@@ -697,8 +635,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8091AE61-1262-4037-83F4-4010979AF21E}">
   <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -741,10 +679,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C4" t="s">
         <v>5</v>
@@ -752,10 +690,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>29</v>
       </c>
       <c r="C5" t="s">
         <v>5</v>
@@ -763,10 +701,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>30</v>
       </c>
       <c r="C6" t="s">
         <v>5</v>
@@ -774,21 +712,21 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>3</v>
+        <v>31</v>
       </c>
       <c r="C7" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>9</v>
+        <v>32</v>
       </c>
       <c r="C8" t="s">
         <v>5</v>
@@ -796,10 +734,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>30</v>
       </c>
       <c r="B9" t="s">
-        <v>11</v>
+        <v>33</v>
       </c>
       <c r="C9" t="s">
         <v>5</v>
@@ -807,32 +745,32 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="B10" t="s">
-        <v>6</v>
+        <v>33</v>
       </c>
       <c r="C10" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B11" t="s">
-        <v>4</v>
+        <v>33</v>
       </c>
       <c r="C11" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="B12" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C12" t="s">
         <v>5</v>
@@ -840,24 +778,215 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C13" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B14" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="C14" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C15" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>35</v>
+      </c>
+      <c r="B17" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>35</v>
+      </c>
+      <c r="B18" t="s">
+        <v>31</v>
+      </c>
+      <c r="C18" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>35</v>
+      </c>
+      <c r="B19" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C3897CC-5AFD-43BB-81EC-925537313582}">
+  <dimension ref="A4:C38"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A21" sqref="A21:C38"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
@@ -865,43 +994,43 @@
         <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="C15" t="s">
-        <v>5</v>
+        <v>25</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B16" t="s">
-        <v>3</v>
+        <v>22</v>
       </c>
       <c r="C16" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B17" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="C17" t="s">
-        <v>5</v>
+        <v>25</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="C18" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
@@ -909,10 +1038,208 @@
         <v>28</v>
       </c>
       <c r="B19" t="s">
+        <v>24</v>
+      </c>
+      <c r="C19" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>3</v>
+      </c>
+      <c r="B22" t="s">
+        <v>4</v>
+      </c>
+      <c r="C22" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>4</v>
+      </c>
+      <c r="B23" t="s">
+        <v>6</v>
+      </c>
+      <c r="C23" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>6</v>
+      </c>
+      <c r="B24" t="s">
+        <v>7</v>
+      </c>
+      <c r="C24" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>6</v>
+      </c>
+      <c r="B25" t="s">
+        <v>8</v>
+      </c>
+      <c r="C25" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>7</v>
+      </c>
+      <c r="B26" t="s">
+        <v>9</v>
+      </c>
+      <c r="C26" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>9</v>
+      </c>
+      <c r="B27" t="s">
+        <v>3</v>
+      </c>
+      <c r="C27" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>8</v>
+      </c>
+      <c r="B28" t="s">
+        <v>9</v>
+      </c>
+      <c r="C28" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>8</v>
+      </c>
+      <c r="B29" t="s">
+        <v>11</v>
+      </c>
+      <c r="C29" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>12</v>
+      </c>
+      <c r="B30" t="s">
+        <v>6</v>
+      </c>
+      <c r="C30" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>12</v>
+      </c>
+      <c r="B31" t="s">
+        <v>4</v>
+      </c>
+      <c r="C31" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
         <v>13</v>
       </c>
-      <c r="C19" t="s">
-        <v>5</v>
+      <c r="B32" t="s">
+        <v>14</v>
+      </c>
+      <c r="C32" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>14</v>
+      </c>
+      <c r="B33" t="s">
+        <v>3</v>
+      </c>
+      <c r="C33" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>15</v>
+      </c>
+      <c r="B34" t="s">
+        <v>14</v>
+      </c>
+      <c r="C34" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>15</v>
+      </c>
+      <c r="B35" t="s">
+        <v>16</v>
+      </c>
+      <c r="C35" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>16</v>
+      </c>
+      <c r="B36" t="s">
+        <v>3</v>
+      </c>
+      <c r="C36" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>17</v>
+      </c>
+      <c r="B37" t="s">
+        <v>15</v>
+      </c>
+      <c r="C37" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>18</v>
+      </c>
+      <c r="B38" t="s">
+        <v>3</v>
+      </c>
+      <c r="C38" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>